<commit_message>
fix to WCU rate
</commit_message>
<xml_diff>
--- a/DynamoDB - Reserved Capacity Cost Calculator.xlsx
+++ b/DynamoDB - Reserved Capacity Cost Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werberm/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmebham/Documents/AWS/general/cost optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86171E2D-9A54-7243-88FD-E785EBDBC64E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A7AFA9D-65E8-F54D-813A-A141B81B2DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{955865D9-57C2-E04D-998A-D98083884EBC}"/>
+    <workbookView xWindow="2880" yWindow="2300" windowWidth="28800" windowHeight="14120" xr2:uid="{955865D9-57C2-E04D-998A-D98083884EBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Metrics" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>Hour</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Averages:</t>
+  </si>
+  <si>
+    <t>Total monthly cost</t>
+  </si>
+  <si>
+    <t>Total yearly cost</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -698,7 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -736,6 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -757,7 +763,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -766,7 +771,167 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1020,7 +1185,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$B$40</c:f>
+              <c:f>'Daily Metrics'!$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1043,7 +1208,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$B$41:$B$64</c:f>
+              <c:f>'Daily Metrics'!$B$44:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1134,7 +1299,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$C$40</c:f>
+              <c:f>'Daily Metrics'!$C$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1322,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$C$41:$C$64</c:f>
+              <c:f>'Daily Metrics'!$C$44:$C$67</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1248,7 +1413,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$D$40</c:f>
+              <c:f>'Daily Metrics'!$D$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1272,7 +1437,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$D$41:$D$64</c:f>
+              <c:f>'Daily Metrics'!$D$44:$D$67</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1639,7 +1804,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$B$73</c:f>
+              <c:f>'Daily Metrics'!$B$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1662,7 +1827,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$B$74:$B$97</c:f>
+              <c:f>'Daily Metrics'!$B$77:$B$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1753,7 +1918,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$C$73</c:f>
+              <c:f>'Daily Metrics'!$C$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1776,7 +1941,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$C$74:$C$97</c:f>
+              <c:f>'Daily Metrics'!$C$77:$C$100</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1867,7 +2032,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Daily Metrics'!$D$73</c:f>
+              <c:f>'Daily Metrics'!$D$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1891,7 +2056,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily Metrics'!$D$74:$D$97</c:f>
+              <c:f>'Daily Metrics'!$D$77:$D$100</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
@@ -3859,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8865C407-BE62-3B4F-A737-3FBB6D70F36C}">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3899,11 +4064,11 @@
       <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68" t="s">
+      <c r="B22" s="66"/>
+      <c r="C22" s="67" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -3914,7 +4079,7 @@
       <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="26">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3957,7 +4122,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="27" thickBot="1">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="65" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="2"/>
@@ -3966,369 +4131,308 @@
       <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="51" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="F31" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="43" t="s">
+      <c r="G31" s="42" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="52">
-        <f>F68</f>
+      <c r="B32" s="58"/>
+      <c r="C32" s="51">
+        <f>F71</f>
         <v>3.6985000000000001</v>
       </c>
-      <c r="D32" s="44">
-        <f>I68</f>
+      <c r="D32" s="43">
+        <f>I71</f>
         <v>2.5838013698630138</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="44">
         <f>C32-D32</f>
         <v>1.1146986301369863</v>
       </c>
-      <c r="F32" s="44">
-        <f>L68</f>
+      <c r="F32" s="43">
+        <f>L71</f>
         <v>1.7328205479452061</v>
       </c>
-      <c r="G32" s="45">
+      <c r="G32" s="44">
         <f>C32-F32</f>
         <v>1.965679452054794</v>
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="61"/>
-      <c r="C33" s="53">
-        <f>F101</f>
-        <v>7.6569999999999991</v>
-      </c>
-      <c r="D33" s="46">
-        <f>I101</f>
-        <v>4.6622191780821938</v>
-      </c>
-      <c r="E33" s="47">
+      <c r="B33" s="60"/>
+      <c r="C33" s="52">
+        <f>F104</f>
+        <v>38.284999999999997</v>
+      </c>
+      <c r="D33" s="45">
+        <f>I104</f>
+        <v>23.469495890410961</v>
+      </c>
+      <c r="E33" s="46">
         <f>C33-D33</f>
-        <v>2.9947808219178054</v>
-      </c>
-      <c r="F33" s="46">
-        <f>L101</f>
-        <v>3.102087671232876</v>
-      </c>
-      <c r="G33" s="47">
+        <v>14.815504109589035</v>
+      </c>
+      <c r="F33" s="45">
+        <f>L104</f>
+        <v>15.563238356164378</v>
+      </c>
+      <c r="G33" s="46">
         <f>C33-F33</f>
-        <v>4.5549123287671236</v>
+        <v>22.72176164383562</v>
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="63"/>
-      <c r="C34" s="54">
+      <c r="B34" s="62"/>
+      <c r="C34" s="53">
         <f>SUM(C32:C33)</f>
-        <v>11.355499999999999</v>
-      </c>
-      <c r="D34" s="48">
+        <v>41.983499999999999</v>
+      </c>
+      <c r="D34" s="47">
         <f>SUM(D32:D33)</f>
-        <v>7.2460205479452071</v>
-      </c>
-      <c r="E34" s="45">
+        <v>26.053297260273975</v>
+      </c>
+      <c r="E34" s="44">
         <f>C34-D34</f>
-        <v>4.1094794520547921</v>
-      </c>
-      <c r="F34" s="48">
+        <v>15.930202739726024</v>
+      </c>
+      <c r="F34" s="47">
         <f>SUM(F32:F33)</f>
-        <v>4.8349082191780823</v>
-      </c>
-      <c r="G34" s="45">
+        <v>17.296058904109586</v>
+      </c>
+      <c r="G34" s="44">
         <f>C34-F34</f>
-        <v>6.5205917808219169</v>
+        <v>24.687441095890414</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" thickBot="1">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50">
+      <c r="B35" s="64"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49">
         <f>E34/C34</f>
-        <v>0.36189330738891218</v>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50">
+        <v>0.37943960698193396</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="49">
         <f>G34/C34</f>
-        <v>0.57422322053823405</v>
+        <v>0.58802722726524503</v>
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="G36" s="41"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="3"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="1:12" ht="26">
-      <c r="A38" s="66" t="s">
+      <c r="A36" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="62"/>
+      <c r="C36" s="53">
+        <f>SUM(C34:C35)*30</f>
+        <v>1259.5049999999999</v>
+      </c>
+      <c r="D36" s="53">
+        <f>SUM(D34:D35)*30</f>
+        <v>781.59891780821931</v>
+      </c>
+      <c r="E36" s="44">
+        <f>C36-D36</f>
+        <v>477.90608219178057</v>
+      </c>
+      <c r="F36" s="47">
+        <f>SUM(F34:F35)*30</f>
+        <v>518.88176712328755</v>
+      </c>
+      <c r="G36" s="44">
+        <f>C36-F36</f>
+        <v>740.62323287671234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="17" thickBot="1">
+      <c r="A37" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="64"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="49">
+        <f>E36/C36</f>
+        <v>0.37943960698193385</v>
+      </c>
+      <c r="F37" s="48"/>
+      <c r="G37" s="49">
+        <f>G36/C36</f>
+        <v>0.58802722726524503</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="62"/>
+      <c r="C38" s="53">
+        <f>SUM(C36:C37)*12</f>
+        <v>15114.059999999998</v>
+      </c>
+      <c r="D38" s="53">
+        <f>SUM(D36:D37)*12</f>
+        <v>9379.1870136986327</v>
+      </c>
+      <c r="E38" s="44">
+        <f>C38-D38</f>
+        <v>5734.872986301365</v>
+      </c>
+      <c r="F38" s="47">
+        <f>SUM(F36:F37)*12</f>
+        <v>6226.5812054794505</v>
+      </c>
+      <c r="G38" s="44">
+        <f>C38-F38</f>
+        <v>8887.4787945205462</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="17" thickBot="1">
+      <c r="A39" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="64"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49">
+        <f>E38/C38</f>
+        <v>0.37943960698193374</v>
+      </c>
+      <c r="F39" s="48"/>
+      <c r="G39" s="49">
+        <f>G38/C38</f>
+        <v>0.58802722726524492</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:12" ht="26">
+      <c r="A41" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="69" t="s">
+      <c r="C41" s="7"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="69" t="s">
+      <c r="B42" s="70"/>
+      <c r="C42" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="71"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="25" t="s">
+      <c r="D42" s="71"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="72" t="s">
+      <c r="G42" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="H39" s="73"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="72" t="s">
+      <c r="H42" s="73"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="K39" s="73"/>
-      <c r="L39" s="74"/>
-    </row>
-    <row r="40" spans="1:12" s="24" customFormat="1" ht="85">
-      <c r="A40" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="26" t="s">
+      <c r="K42" s="73"/>
+      <c r="L42" s="74"/>
+    </row>
+    <row r="43" spans="1:12" s="24" customFormat="1" ht="85">
+      <c r="A43" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C43" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D43" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E43" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F43" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G43" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H40" s="31" t="s">
+      <c r="H43" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I40" s="30" t="s">
+      <c r="I43" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J40" s="32" t="s">
+      <c r="J43" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="33" t="s">
+      <c r="K43" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="L40" s="34" t="s">
+      <c r="L43" s="34" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="12">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="B41" s="13">
-        <v>200</v>
-      </c>
-      <c r="C41" s="15">
-        <f t="shared" ref="C41:C64" si="0">ROUND(B41/$B$27/50,0)*50</f>
-        <v>350</v>
-      </c>
-      <c r="D41" s="15">
-        <f t="shared" ref="D41:D64" si="1">$C$27</f>
-        <v>1200</v>
-      </c>
-      <c r="E41" s="15">
-        <f>MAX(0,C41-D41)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C41</f>
-        <v>4.5499999999999999E-2</v>
-      </c>
-      <c r="G41" s="19">
-        <f>$D41*'Pricing (us-west-2)'!$C$6</f>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="H41" s="20">
-        <f>$E41*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="19">
-        <f>H41+G41</f>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="J41" s="17">
-        <f>$D41*'Pricing (us-west-2)'!$C$7</f>
-        <v>3.5638356164383565E-2</v>
-      </c>
-      <c r="K41" s="18">
-        <f>$E41*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="17">
-        <f>K41+J41</f>
-        <v>3.5638356164383565E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="12">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="B42" s="13">
-        <v>200</v>
-      </c>
-      <c r="C42" s="15">
-        <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-      <c r="D42" s="15">
-        <f t="shared" si="1"/>
-        <v>1200</v>
-      </c>
-      <c r="E42" s="15">
-        <f t="shared" ref="E42:E64" si="2">MAX(0,C42-D42)</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C42</f>
-        <v>4.5499999999999999E-2</v>
-      </c>
-      <c r="G42" s="19">
-        <f>$D42*'Pricing (us-west-2)'!$C$6</f>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="H42" s="20">
-        <f>$E42*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I42" s="19">
-        <f t="shared" ref="I42:I64" si="3">H42+G42</f>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="J42" s="17">
-        <f>$D42*'Pricing (us-west-2)'!$C$7</f>
-        <v>3.5638356164383565E-2</v>
-      </c>
-      <c r="K42" s="18">
-        <f>$E42*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L42" s="17">
-        <f t="shared" ref="L42:L64" si="4">K42+J42</f>
-        <v>3.5638356164383565E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="12">
-        <v>0.125</v>
-      </c>
-      <c r="B43" s="13">
-        <v>200</v>
-      </c>
-      <c r="C43" s="15">
-        <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-      <c r="D43" s="15">
-        <f t="shared" si="1"/>
-        <v>1200</v>
-      </c>
-      <c r="E43" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C43</f>
-        <v>4.5499999999999999E-2</v>
-      </c>
-      <c r="G43" s="19">
-        <f>$D43*'Pricing (us-west-2)'!$C$6</f>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="H43" s="20">
-        <f>$E43*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="19">
-        <f t="shared" si="3"/>
-        <v>7.1095890410958901E-2</v>
-      </c>
-      <c r="J43" s="17">
-        <f>$D43*'Pricing (us-west-2)'!$C$7</f>
-        <v>3.5638356164383565E-2</v>
-      </c>
-      <c r="K43" s="18">
-        <f>$E43*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L43" s="17">
-        <f t="shared" si="4"/>
-        <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="12">
-        <v>0.16666666666666699</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="B44" s="13">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C44" s="15">
-        <f t="shared" si="0"/>
-        <v>850</v>
+        <f t="shared" ref="C44:C67" si="0">ROUND(B44/$B$27/50,0)*50</f>
+        <v>350</v>
       </c>
       <c r="D44" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D44:D67" si="1">$C$27</f>
         <v>1200</v>
       </c>
       <c r="E44" s="15">
-        <f t="shared" si="2"/>
+        <f>MAX(0,C44-D44)</f>
         <v>0</v>
       </c>
       <c r="F44" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C44</f>
-        <v>0.11049999999999999</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="G44" s="19">
         <f>$D44*'Pricing (us-west-2)'!$C$6</f>
@@ -4339,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="19">
-        <f t="shared" si="3"/>
+        <f>H44+G44</f>
         <v>7.1095890410958901E-2</v>
       </c>
       <c r="J44" s="17">
@@ -4351,32 +4455,32 @@
         <v>0</v>
       </c>
       <c r="L44" s="17">
-        <f t="shared" si="4"/>
+        <f>K44+J44</f>
         <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="12">
-        <v>0.20833333333333301</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="B45" s="13">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C45" s="15">
         <f t="shared" si="0"/>
-        <v>850</v>
+        <v>350</v>
       </c>
       <c r="D45" s="15">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
       <c r="E45" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E45:E67" si="2">MAX(0,C45-D45)</f>
         <v>0</v>
       </c>
       <c r="F45" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C45</f>
-        <v>0.11049999999999999</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="G45" s="19">
         <f>$D45*'Pricing (us-west-2)'!$C$6</f>
@@ -4387,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I45:I67" si="3">H45+G45</f>
         <v>7.1095890410958901E-2</v>
       </c>
       <c r="J45" s="17">
@@ -4399,20 +4503,20 @@
         <v>0</v>
       </c>
       <c r="L45" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L45:L67" si="4">K45+J45</f>
         <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="12">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="B46" s="13">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="C46" s="15">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>350</v>
       </c>
       <c r="D46" s="15">
         <f t="shared" si="1"/>
@@ -4420,11 +4524,11 @@
       </c>
       <c r="E46" s="15">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="F46" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C46</f>
-        <v>0.17549999999999999</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="G46" s="19">
         <f>$D46*'Pricing (us-west-2)'!$C$6</f>
@@ -4432,11 +4536,11 @@
       </c>
       <c r="H46" s="20">
         <f>$E46*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0</v>
       </c>
       <c r="I46" s="19">
         <f t="shared" si="3"/>
-        <v>9.0595890410958904E-2</v>
+        <v>7.1095890410958901E-2</v>
       </c>
       <c r="J46" s="17">
         <f>$D46*'Pricing (us-west-2)'!$C$7</f>
@@ -4444,23 +4548,23 @@
       </c>
       <c r="K46" s="18">
         <f>$E46*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="4"/>
-        <v>5.5138356164383562E-2</v>
+        <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="12">
-        <v>0.29166666666666702</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="B47" s="13">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="C47" s="15">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>850</v>
       </c>
       <c r="D47" s="15">
         <f t="shared" si="1"/>
@@ -4468,11 +4572,11 @@
       </c>
       <c r="E47" s="15">
         <f t="shared" si="2"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F47" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C47</f>
-        <v>0.25999999999999995</v>
+        <v>0.11049999999999999</v>
       </c>
       <c r="G47" s="19">
         <f>$D47*'Pricing (us-west-2)'!$C$6</f>
@@ -4480,11 +4584,11 @@
       </c>
       <c r="H47" s="20">
         <f>$E47*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <v>0</v>
       </c>
       <c r="I47" s="19">
         <f t="shared" si="3"/>
-        <v>0.17509589041095891</v>
+        <v>7.1095890410958901E-2</v>
       </c>
       <c r="J47" s="17">
         <f>$D47*'Pricing (us-west-2)'!$C$7</f>
@@ -4492,23 +4596,23 @@
       </c>
       <c r="K47" s="18">
         <f>$E47*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <v>0</v>
       </c>
       <c r="L47" s="17">
         <f t="shared" si="4"/>
-        <v>0.13963835616438355</v>
+        <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="12">
-        <v>0.33333333333333298</v>
+        <v>0.20833333333333301</v>
       </c>
       <c r="B48" s="13">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="C48" s="15">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>850</v>
       </c>
       <c r="D48" s="15">
         <f t="shared" si="1"/>
@@ -4516,11 +4620,11 @@
       </c>
       <c r="E48" s="15">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="F48" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C48</f>
-        <v>0.32499999999999996</v>
+        <v>0.11049999999999999</v>
       </c>
       <c r="G48" s="19">
         <f>$D48*'Pricing (us-west-2)'!$C$6</f>
@@ -4528,11 +4632,11 @@
       </c>
       <c r="H48" s="20">
         <f>$E48*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.16899999999999998</v>
+        <v>0</v>
       </c>
       <c r="I48" s="19">
         <f t="shared" si="3"/>
-        <v>0.24009589041095888</v>
+        <v>7.1095890410958901E-2</v>
       </c>
       <c r="J48" s="17">
         <f>$D48*'Pricing (us-west-2)'!$C$7</f>
@@ -4540,23 +4644,23 @@
       </c>
       <c r="K48" s="18">
         <f>$E48*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.16899999999999998</v>
+        <v>0</v>
       </c>
       <c r="L48" s="17">
         <f t="shared" si="4"/>
-        <v>0.20463835616438356</v>
+        <v>3.5638356164383565E-2</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="12">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="B49" s="13">
-        <v>1600</v>
+        <v>800</v>
       </c>
       <c r="C49" s="15">
         <f t="shared" si="0"/>
-        <v>2650</v>
+        <v>1350</v>
       </c>
       <c r="D49" s="15">
         <f t="shared" si="1"/>
@@ -4564,11 +4668,11 @@
       </c>
       <c r="E49" s="15">
         <f t="shared" si="2"/>
-        <v>1450</v>
+        <v>150</v>
       </c>
       <c r="F49" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C49</f>
-        <v>0.34449999999999997</v>
+        <v>0.17549999999999999</v>
       </c>
       <c r="G49" s="19">
         <f>$D49*'Pricing (us-west-2)'!$C$6</f>
@@ -4576,11 +4680,11 @@
       </c>
       <c r="H49" s="20">
         <f>$E49*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.18849999999999997</v>
+        <v>1.95E-2</v>
       </c>
       <c r="I49" s="19">
         <f t="shared" si="3"/>
-        <v>0.25959589041095887</v>
+        <v>9.0595890410958904E-2</v>
       </c>
       <c r="J49" s="17">
         <f>$D49*'Pricing (us-west-2)'!$C$7</f>
@@ -4588,23 +4692,23 @@
       </c>
       <c r="K49" s="18">
         <f>$E49*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.18849999999999997</v>
+        <v>1.95E-2</v>
       </c>
       <c r="L49" s="17">
         <f t="shared" si="4"/>
-        <v>0.22413835616438355</v>
+        <v>5.5138356164383562E-2</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="12">
-        <v>0.41666666666666702</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="B50" s="13">
-        <v>1700</v>
+        <v>1200</v>
       </c>
       <c r="C50" s="15">
         <f t="shared" si="0"/>
-        <v>2850</v>
+        <v>2000</v>
       </c>
       <c r="D50" s="15">
         <f t="shared" si="1"/>
@@ -4612,11 +4716,11 @@
       </c>
       <c r="E50" s="15">
         <f t="shared" si="2"/>
-        <v>1650</v>
+        <v>800</v>
       </c>
       <c r="F50" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C50</f>
-        <v>0.37049999999999994</v>
+        <v>0.25999999999999995</v>
       </c>
       <c r="G50" s="19">
         <f>$D50*'Pricing (us-west-2)'!$C$6</f>
@@ -4624,11 +4728,11 @@
       </c>
       <c r="H50" s="20">
         <f>$E50*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.21449999999999997</v>
+        <v>0.104</v>
       </c>
       <c r="I50" s="19">
         <f t="shared" si="3"/>
-        <v>0.2855958904109589</v>
+        <v>0.17509589041095891</v>
       </c>
       <c r="J50" s="17">
         <f>$D50*'Pricing (us-west-2)'!$C$7</f>
@@ -4636,23 +4740,23 @@
       </c>
       <c r="K50" s="18">
         <f>$E50*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.21449999999999997</v>
+        <v>0.104</v>
       </c>
       <c r="L50" s="17">
         <f t="shared" si="4"/>
-        <v>0.25013835616438351</v>
+        <v>0.13963835616438355</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="12">
-        <v>0.45833333333333298</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="B51" s="13">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="C51" s="15">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="D51" s="15">
         <f t="shared" si="1"/>
@@ -4660,11 +4764,11 @@
       </c>
       <c r="E51" s="15">
         <f t="shared" si="2"/>
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="F51" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C51</f>
-        <v>0.25999999999999995</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="G51" s="19">
         <f>$D51*'Pricing (us-west-2)'!$C$6</f>
@@ -4672,11 +4776,11 @@
       </c>
       <c r="H51" s="20">
         <f>$E51*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <v>0.16899999999999998</v>
       </c>
       <c r="I51" s="19">
         <f t="shared" si="3"/>
-        <v>0.17509589041095891</v>
+        <v>0.24009589041095888</v>
       </c>
       <c r="J51" s="17">
         <f>$D51*'Pricing (us-west-2)'!$C$7</f>
@@ -4684,23 +4788,23 @@
       </c>
       <c r="K51" s="18">
         <f>$E51*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <v>0.16899999999999998</v>
       </c>
       <c r="L51" s="17">
         <f t="shared" si="4"/>
-        <v>0.13963835616438355</v>
+        <v>0.20463835616438356</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="12">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="B52" s="13">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="C52" s="15">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>2650</v>
       </c>
       <c r="D52" s="15">
         <f t="shared" si="1"/>
@@ -4708,11 +4812,11 @@
       </c>
       <c r="E52" s="15">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>1450</v>
       </c>
       <c r="F52" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C52</f>
-        <v>0.17549999999999999</v>
+        <v>0.34449999999999997</v>
       </c>
       <c r="G52" s="19">
         <f>$D52*'Pricing (us-west-2)'!$C$6</f>
@@ -4720,11 +4824,11 @@
       </c>
       <c r="H52" s="20">
         <f>$E52*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.18849999999999997</v>
       </c>
       <c r="I52" s="19">
         <f t="shared" si="3"/>
-        <v>9.0595890410958904E-2</v>
+        <v>0.25959589041095887</v>
       </c>
       <c r="J52" s="17">
         <f>$D52*'Pricing (us-west-2)'!$C$7</f>
@@ -4732,23 +4836,23 @@
       </c>
       <c r="K52" s="18">
         <f>$E52*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.18849999999999997</v>
       </c>
       <c r="L52" s="17">
         <f t="shared" si="4"/>
-        <v>5.5138356164383562E-2</v>
+        <v>0.22413835616438355</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="12">
-        <v>0.54166666666666696</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="B53" s="13">
-        <v>800</v>
+        <v>1700</v>
       </c>
       <c r="C53" s="15">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>2850</v>
       </c>
       <c r="D53" s="15">
         <f t="shared" si="1"/>
@@ -4756,11 +4860,11 @@
       </c>
       <c r="E53" s="15">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>1650</v>
       </c>
       <c r="F53" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C53</f>
-        <v>0.17549999999999999</v>
+        <v>0.37049999999999994</v>
       </c>
       <c r="G53" s="19">
         <f>$D53*'Pricing (us-west-2)'!$C$6</f>
@@ -4768,11 +4872,11 @@
       </c>
       <c r="H53" s="20">
         <f>$E53*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.21449999999999997</v>
       </c>
       <c r="I53" s="19">
         <f t="shared" si="3"/>
-        <v>9.0595890410958904E-2</v>
+        <v>0.2855958904109589</v>
       </c>
       <c r="J53" s="17">
         <f>$D53*'Pricing (us-west-2)'!$C$7</f>
@@ -4780,23 +4884,23 @@
       </c>
       <c r="K53" s="18">
         <f>$E53*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.21449999999999997</v>
       </c>
       <c r="L53" s="17">
         <f t="shared" si="4"/>
-        <v>5.5138356164383562E-2</v>
+        <v>0.25013835616438351</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="12">
-        <v>0.58333333333333304</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="B54" s="13">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="C54" s="15">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>2000</v>
       </c>
       <c r="D54" s="15">
         <f t="shared" si="1"/>
@@ -4804,11 +4908,11 @@
       </c>
       <c r="E54" s="15">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>800</v>
       </c>
       <c r="F54" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C54</f>
-        <v>0.17549999999999999</v>
+        <v>0.25999999999999995</v>
       </c>
       <c r="G54" s="19">
         <f>$D54*'Pricing (us-west-2)'!$C$6</f>
@@ -4816,11 +4920,11 @@
       </c>
       <c r="H54" s="20">
         <f>$E54*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.104</v>
       </c>
       <c r="I54" s="19">
         <f t="shared" si="3"/>
-        <v>9.0595890410958904E-2</v>
+        <v>0.17509589041095891</v>
       </c>
       <c r="J54" s="17">
         <f>$D54*'Pricing (us-west-2)'!$C$7</f>
@@ -4828,16 +4932,16 @@
       </c>
       <c r="K54" s="18">
         <f>$E54*'Pricing (us-west-2)'!$C$5</f>
-        <v>1.95E-2</v>
+        <v>0.104</v>
       </c>
       <c r="L54" s="17">
         <f t="shared" si="4"/>
-        <v>5.5138356164383562E-2</v>
+        <v>0.13963835616438355</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="12">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="B55" s="13">
         <v>800</v>
@@ -4885,14 +4989,14 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="12">
-        <v>0.66666666666666696</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="B56" s="13">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="C56" s="15">
         <f t="shared" si="0"/>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="D56" s="15">
         <f t="shared" si="1"/>
@@ -4900,11 +5004,11 @@
       </c>
       <c r="E56" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F56" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C56</f>
-        <v>0.14949999999999999</v>
+        <v>0.17549999999999999</v>
       </c>
       <c r="G56" s="19">
         <f>$D56*'Pricing (us-west-2)'!$C$6</f>
@@ -4912,11 +5016,11 @@
       </c>
       <c r="H56" s="20">
         <f>$E56*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="I56" s="19">
         <f t="shared" si="3"/>
-        <v>7.1095890410958901E-2</v>
+        <v>9.0595890410958904E-2</v>
       </c>
       <c r="J56" s="17">
         <f>$D56*'Pricing (us-west-2)'!$C$7</f>
@@ -4924,23 +5028,23 @@
       </c>
       <c r="K56" s="18">
         <f>$E56*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="L56" s="17">
         <f t="shared" si="4"/>
-        <v>3.5638356164383565E-2</v>
+        <v>5.5138356164383562E-2</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="12">
-        <v>0.70833333333333304</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="B57" s="13">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="C57" s="15">
         <f t="shared" si="0"/>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="D57" s="15">
         <f t="shared" si="1"/>
@@ -4948,11 +5052,11 @@
       </c>
       <c r="E57" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F57" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C57</f>
-        <v>0.14949999999999999</v>
+        <v>0.17549999999999999</v>
       </c>
       <c r="G57" s="19">
         <f>$D57*'Pricing (us-west-2)'!$C$6</f>
@@ -4960,11 +5064,11 @@
       </c>
       <c r="H57" s="20">
         <f>$E57*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="I57" s="19">
         <f t="shared" si="3"/>
-        <v>7.1095890410958901E-2</v>
+        <v>9.0595890410958904E-2</v>
       </c>
       <c r="J57" s="17">
         <f>$D57*'Pricing (us-west-2)'!$C$7</f>
@@ -4972,23 +5076,23 @@
       </c>
       <c r="K57" s="18">
         <f>$E57*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="L57" s="17">
         <f t="shared" si="4"/>
-        <v>3.5638356164383565E-2</v>
+        <v>5.5138356164383562E-2</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="12">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="B58" s="13">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="C58" s="15">
         <f t="shared" si="0"/>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="D58" s="15">
         <f t="shared" si="1"/>
@@ -4996,11 +5100,11 @@
       </c>
       <c r="E58" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F58" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C58</f>
-        <v>0.14949999999999999</v>
+        <v>0.17549999999999999</v>
       </c>
       <c r="G58" s="19">
         <f>$D58*'Pricing (us-west-2)'!$C$6</f>
@@ -5008,11 +5112,11 @@
       </c>
       <c r="H58" s="20">
         <f>$E58*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="I58" s="19">
         <f t="shared" si="3"/>
-        <v>7.1095890410958901E-2</v>
+        <v>9.0595890410958904E-2</v>
       </c>
       <c r="J58" s="17">
         <f>$D58*'Pricing (us-west-2)'!$C$7</f>
@@ -5020,16 +5124,16 @@
       </c>
       <c r="K58" s="18">
         <f>$E58*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <v>1.95E-2</v>
       </c>
       <c r="L58" s="17">
         <f t="shared" si="4"/>
-        <v>3.5638356164383565E-2</v>
+        <v>5.5138356164383562E-2</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="12">
-        <v>0.79166666666666696</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="B59" s="13">
         <v>700</v>
@@ -5077,14 +5181,14 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="12">
-        <v>0.83333333333333304</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="B60" s="13">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="C60" s="15">
         <f t="shared" si="0"/>
-        <v>650</v>
+        <v>1150</v>
       </c>
       <c r="D60" s="15">
         <f t="shared" si="1"/>
@@ -5096,7 +5200,7 @@
       </c>
       <c r="F60" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C60</f>
-        <v>8.4499999999999992E-2</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="G60" s="19">
         <f>$D60*'Pricing (us-west-2)'!$C$6</f>
@@ -5125,14 +5229,14 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="12">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="B61" s="13">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="C61" s="15">
         <f t="shared" si="0"/>
-        <v>650</v>
+        <v>1150</v>
       </c>
       <c r="D61" s="15">
         <f t="shared" si="1"/>
@@ -5144,7 +5248,7 @@
       </c>
       <c r="F61" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C61</f>
-        <v>8.4499999999999992E-2</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="G61" s="19">
         <f>$D61*'Pricing (us-west-2)'!$C$6</f>
@@ -5173,14 +5277,14 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="12">
-        <v>0.91666666666666596</v>
+        <v>0.79166666666666696</v>
       </c>
       <c r="B62" s="13">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="C62" s="15">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>1150</v>
       </c>
       <c r="D62" s="15">
         <f t="shared" si="1"/>
@@ -5192,7 +5296,7 @@
       </c>
       <c r="F62" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C62</f>
-        <v>4.5499999999999999E-2</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="G62" s="19">
         <f>$D62*'Pricing (us-west-2)'!$C$6</f>
@@ -5221,14 +5325,14 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="12">
-        <v>0.95833333333333304</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="B63" s="13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C63" s="15">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="D63" s="15">
         <f t="shared" si="1"/>
@@ -5240,7 +5344,7 @@
       </c>
       <c r="F63" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C63</f>
-        <v>4.5499999999999999E-2</v>
+        <v>8.4499999999999992E-2</v>
       </c>
       <c r="G63" s="19">
         <f>$D63*'Pricing (us-west-2)'!$C$6</f>
@@ -5269,14 +5373,14 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="12">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="B64" s="13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C64" s="15">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="D64" s="15">
         <f t="shared" si="1"/>
@@ -5288,7 +5392,7 @@
       </c>
       <c r="F64" s="21">
         <f>'Pricing (us-west-2)'!$C$5*C64</f>
-        <v>4.5499999999999999E-2</v>
+        <v>8.4499999999999992E-2</v>
       </c>
       <c r="G64" s="19">
         <f>$D64*'Pricing (us-west-2)'!$C$6</f>
@@ -5315,373 +5419,373 @@
         <v>3.5638356164383565E-2</v>
       </c>
     </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="12">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="B65" s="13">
+        <v>200</v>
+      </c>
+      <c r="C65" s="15">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="D65" s="15">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="E65" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="21">
+        <f>'Pricing (us-west-2)'!$C$5*C65</f>
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="G65" s="19">
+        <f>$D65*'Pricing (us-west-2)'!$C$6</f>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="H65" s="20">
+        <f>$E65*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="I65" s="19">
+        <f t="shared" si="3"/>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="J65" s="17">
+        <f>$D65*'Pricing (us-west-2)'!$C$7</f>
+        <v>3.5638356164383565E-2</v>
+      </c>
+      <c r="K65" s="18">
+        <f>$E65*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="L65" s="17">
+        <f t="shared" si="4"/>
+        <v>3.5638356164383565E-2</v>
+      </c>
+    </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="12">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B66" s="13">
+        <v>200</v>
+      </c>
+      <c r="C66" s="15">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="D66" s="15">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="E66" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="21">
+        <f>'Pricing (us-west-2)'!$C$5*C66</f>
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="G66" s="19">
+        <f>$D66*'Pricing (us-west-2)'!$C$6</f>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="H66" s="20">
+        <f>$E66*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="19">
+        <f t="shared" si="3"/>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="J66" s="17">
+        <f>$D66*'Pricing (us-west-2)'!$C$7</f>
+        <v>3.5638356164383565E-2</v>
+      </c>
+      <c r="K66" s="18">
+        <f>$E66*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="L66" s="17">
+        <f t="shared" si="4"/>
+        <v>3.5638356164383565E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="12">
+        <v>1</v>
+      </c>
+      <c r="B67" s="13">
+        <v>200</v>
+      </c>
+      <c r="C67" s="15">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="D67" s="15">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="E67" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="21">
+        <f>'Pricing (us-west-2)'!$C$5*C67</f>
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="G67" s="19">
+        <f>$D67*'Pricing (us-west-2)'!$C$6</f>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="H67" s="20">
+        <f>$E67*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="19">
+        <f t="shared" si="3"/>
+        <v>7.1095890410958901E-2</v>
+      </c>
+      <c r="J67" s="17">
+        <f>$D67*'Pricing (us-west-2)'!$C$7</f>
+        <v>3.5638356164383565E-2</v>
+      </c>
+      <c r="K67" s="18">
+        <f>$E67*'Pricing (us-west-2)'!$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="L67" s="17">
+        <f t="shared" si="4"/>
+        <v>3.5638356164383565E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="76">
-        <f>AVERAGE(B41:B64)</f>
+      <c r="B69" s="68">
+        <f>AVERAGE(B44:B67)</f>
         <v>708.33333333333337</v>
       </c>
-      <c r="C66" s="76">
-        <f>AVERAGE(C41:C64)</f>
+      <c r="C69" s="68">
+        <f>AVERAGE(C44:C67)</f>
         <v>1185.4166666666667</v>
       </c>
-      <c r="D66" s="76">
-        <f>AVERAGE(D41:D64)</f>
+      <c r="D69" s="68">
+        <f>AVERAGE(D44:D67)</f>
         <v>1200</v>
       </c>
-      <c r="E66" s="76">
-        <f>AVERAGE(E41:E64)</f>
+      <c r="E69" s="68">
+        <f>AVERAGE(E44:E67)</f>
         <v>281.25</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="22" t="s">
+    <row r="71" spans="1:12">
+      <c r="A71" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22">
-        <f>SUM(F41:F64)</f>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22">
+        <f>SUM(F44:F67)</f>
         <v>3.6985000000000001</v>
       </c>
-      <c r="G68" s="22"/>
-      <c r="H68" s="22" t="s">
+      <c r="G71" s="22"/>
+      <c r="H71" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I68" s="22">
-        <f>SUM(I41:I64)</f>
+      <c r="I71" s="22">
+        <f>SUM(I44:I67)</f>
         <v>2.5838013698630138</v>
       </c>
-      <c r="J68" s="22"/>
-      <c r="K68" s="22" t="s">
+      <c r="J71" s="22"/>
+      <c r="K71" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="L68" s="22">
-        <f>SUM(L41:L64)</f>
+      <c r="L71" s="22">
+        <f>SUM(L44:L67)</f>
         <v>1.7328205479452061</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="26">
-      <c r="A71" s="66" t="s">
+    <row r="74" spans="1:12" ht="26">
+      <c r="A74" s="65" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="69" t="s">
+    <row r="75" spans="1:12">
+      <c r="A75" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="70"/>
-      <c r="C72" s="69" t="s">
+      <c r="B75" s="70"/>
+      <c r="C75" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="D72" s="71"/>
-      <c r="E72" s="70"/>
-      <c r="F72" s="25" t="s">
+      <c r="D75" s="71"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="G72" s="72" t="s">
+      <c r="G75" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="H72" s="73"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="72" t="s">
+      <c r="H75" s="73"/>
+      <c r="I75" s="74"/>
+      <c r="J75" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="K72" s="73"/>
-      <c r="L72" s="74"/>
-    </row>
-    <row r="73" spans="1:12" ht="85">
-      <c r="A73" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="26" t="s">
+      <c r="K75" s="73"/>
+      <c r="L75" s="74"/>
+    </row>
+    <row r="76" spans="1:12" ht="85">
+      <c r="A76" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="27" t="s">
+      <c r="C76" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D73" s="27" t="s">
+      <c r="D76" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E73" s="28" t="s">
+      <c r="E76" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F73" s="29" t="s">
+      <c r="F76" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G73" s="30" t="s">
+      <c r="G76" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H73" s="31" t="s">
+      <c r="H76" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I73" s="30" t="s">
+      <c r="I76" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J73" s="32" t="s">
+      <c r="J76" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K73" s="33" t="s">
+      <c r="K76" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="L73" s="34" t="s">
+      <c r="L76" s="34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="14">
+    <row r="77" spans="1:12">
+      <c r="A77" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="B74" s="13">
+      <c r="B77" s="13">
         <v>1100</v>
       </c>
-      <c r="C74" s="15">
-        <f t="shared" ref="C74:C97" si="5">ROUND(B74/$B$28/50,0)*50</f>
+      <c r="C77" s="15">
+        <f t="shared" ref="C77:C100" si="5">ROUND(B77/$B$28/50,0)*50</f>
         <v>2200</v>
       </c>
-      <c r="D74" s="15">
-        <f t="shared" ref="D74:D97" si="6">$C$28</f>
+      <c r="D77" s="15">
+        <f t="shared" ref="D77:D100" si="6">$C$28</f>
         <v>2200</v>
       </c>
-      <c r="E74" s="15">
-        <f>MAX(0,C74-D74)</f>
-        <v>0</v>
-      </c>
-      <c r="F74" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C74</f>
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="G74" s="19">
-        <f>$D74*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="H74" s="20">
-        <f>$E74*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I74" s="19">
-        <f>H74+G74</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="J74" s="17">
-        <f>$D74*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-      <c r="K74" s="18">
-        <f>$E74*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L74" s="17">
-        <f>K74+J74</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="A75" s="14">
+      <c r="E77" s="15">
+        <f>MAX(0,C77-D77)</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="21">
+        <f>'Pricing (us-west-2)'!$B$5*C77</f>
+        <v>1.43</v>
+      </c>
+      <c r="G77" s="19">
+        <f>$D77*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="H77" s="20">
+        <f>$E77*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="I77" s="19">
+        <f>H77+G77</f>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="J77" s="17">
+        <f>$D77*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
+      </c>
+      <c r="K77" s="18">
+        <f>$E77*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="L77" s="17">
+        <f>K77+J77</f>
+        <v>0.32888493150684928</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B75" s="13">
+      <c r="B78" s="13">
         <v>1100</v>
       </c>
-      <c r="C75" s="15">
+      <c r="C78" s="15">
         <f t="shared" si="5"/>
         <v>2200</v>
-      </c>
-      <c r="D75" s="15">
-        <f t="shared" si="6"/>
-        <v>2200</v>
-      </c>
-      <c r="E75" s="15">
-        <f t="shared" ref="E75:E97" si="7">MAX(0,C75-D75)</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C75</f>
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="G75" s="19">
-        <f>$D75*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="H75" s="20">
-        <f>$E75*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I75" s="19">
-        <f t="shared" ref="I75:I97" si="8">H75+G75</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="J75" s="17">
-        <f>$D75*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-      <c r="K75" s="18">
-        <f>$E75*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L75" s="17">
-        <f t="shared" ref="L75:L97" si="9">K75+J75</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="14">
-        <v>0.125</v>
-      </c>
-      <c r="B76" s="13">
-        <v>1100</v>
-      </c>
-      <c r="C76" s="15">
-        <f t="shared" si="5"/>
-        <v>2200</v>
-      </c>
-      <c r="D76" s="15">
-        <f t="shared" si="6"/>
-        <v>2200</v>
-      </c>
-      <c r="E76" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F76" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C76</f>
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="G76" s="19">
-        <f>$D76*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="H76" s="20">
-        <f>$E76*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I76" s="19">
-        <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="J76" s="17">
-        <f>$D76*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-      <c r="K76" s="18">
-        <f>$E76*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L76" s="17">
-        <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="14">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="B77" s="13">
-        <v>1100</v>
-      </c>
-      <c r="C77" s="15">
-        <f t="shared" si="5"/>
-        <v>2200</v>
-      </c>
-      <c r="D77" s="15">
-        <f t="shared" si="6"/>
-        <v>2200</v>
-      </c>
-      <c r="E77" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F77" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C77</f>
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="G77" s="19">
-        <f>$D77*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="H77" s="20">
-        <f>$E77*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="19">
-        <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
-      </c>
-      <c r="J77" s="17">
-        <f>$D77*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
-      </c>
-      <c r="K77" s="18">
-        <f>$E77*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
-      </c>
-      <c r="L77" s="17">
-        <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="14">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="B78" s="13">
-        <v>1500</v>
-      </c>
-      <c r="C78" s="15">
-        <f t="shared" si="5"/>
-        <v>3000</v>
       </c>
       <c r="D78" s="15">
         <f t="shared" si="6"/>
         <v>2200</v>
       </c>
       <c r="E78" s="15">
-        <f t="shared" si="7"/>
-        <v>800</v>
+        <f t="shared" ref="E78:E100" si="7">MAX(0,C78-D78)</f>
+        <v>0</v>
       </c>
       <c r="F78" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C78</f>
-        <v>0.38999999999999996</v>
+        <f>'Pricing (us-west-2)'!$B$5*C78</f>
+        <v>1.43</v>
       </c>
       <c r="G78" s="19">
-        <f>$D78*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D78*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H78" s="20">
-        <f>$E78*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <f>$E78*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I78" s="19">
-        <f t="shared" si="8"/>
-        <v>0.23434246575342466</v>
+        <f t="shared" ref="I78:I100" si="8">H78+G78</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J78" s="17">
-        <f>$D78*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D78*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K78" s="18">
-        <f>$E78*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <f>$E78*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L78" s="17">
-        <f t="shared" si="9"/>
-        <v>0.16933698630136987</v>
+        <f t="shared" ref="L78:L100" si="9">K78+J78</f>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="14">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="B79" s="13">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="C79" s="15">
         <f t="shared" si="5"/>
-        <v>3600</v>
+        <v>2200</v>
       </c>
       <c r="D79" s="15">
         <f t="shared" si="6"/>
@@ -5689,47 +5793,47 @@
       </c>
       <c r="E79" s="15">
         <f t="shared" si="7"/>
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="F79" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C79</f>
-        <v>0.46799999999999997</v>
+        <f>'Pricing (us-west-2)'!$B$5*C79</f>
+        <v>1.43</v>
       </c>
       <c r="G79" s="19">
-        <f>$D79*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D79*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H79" s="20">
-        <f>$E79*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.182</v>
+        <f>$E79*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I79" s="19">
         <f t="shared" si="8"/>
-        <v>0.31234246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J79" s="17">
-        <f>$D79*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D79*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K79" s="18">
-        <f>$E79*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.182</v>
+        <f>$E79*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L79" s="17">
         <f t="shared" si="9"/>
-        <v>0.24733698630136985</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="14">
-        <v>0.29166666666666702</v>
+        <v>0.16666666666666699</v>
       </c>
       <c r="B80" s="13">
-        <v>1500</v>
+        <v>1100</v>
       </c>
       <c r="C80" s="15">
         <f t="shared" si="5"/>
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="D80" s="15">
         <f t="shared" si="6"/>
@@ -5737,47 +5841,47 @@
       </c>
       <c r="E80" s="15">
         <f t="shared" si="7"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F80" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C80</f>
-        <v>0.38999999999999996</v>
+        <f>'Pricing (us-west-2)'!$B$5*C80</f>
+        <v>1.43</v>
       </c>
       <c r="G80" s="19">
-        <f>$D80*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D80*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H80" s="20">
-        <f>$E80*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <f>$E80*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I80" s="19">
         <f t="shared" si="8"/>
-        <v>0.23434246575342466</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J80" s="17">
-        <f>$D80*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D80*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K80" s="18">
-        <f>$E80*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.104</v>
+        <f>$E80*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L80" s="17">
         <f t="shared" si="9"/>
-        <v>0.16933698630136987</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="14">
-        <v>0.33333333333333298</v>
+        <v>0.20833333333333301</v>
       </c>
       <c r="B81" s="13">
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="C81" s="15">
         <f t="shared" si="5"/>
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="D81" s="15">
         <f t="shared" si="6"/>
@@ -5785,47 +5889,47 @@
       </c>
       <c r="E81" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="F81" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C81</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C81</f>
+        <v>1.95</v>
       </c>
       <c r="G81" s="19">
-        <f>$D81*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D81*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H81" s="20">
-        <f>$E81*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E81*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.52</v>
       </c>
       <c r="I81" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>1.1783123287671233</v>
       </c>
       <c r="J81" s="17">
-        <f>$D81*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D81*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K81" s="18">
-        <f>$E81*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E81*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.52</v>
       </c>
       <c r="L81" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.84888493150684929</v>
       </c>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="14">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="B82" s="13">
-        <v>1100</v>
+        <v>1800</v>
       </c>
       <c r="C82" s="15">
         <f t="shared" si="5"/>
-        <v>2200</v>
+        <v>3600</v>
       </c>
       <c r="D82" s="15">
         <f t="shared" si="6"/>
@@ -5833,47 +5937,47 @@
       </c>
       <c r="E82" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="F82" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C82</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C82</f>
+        <v>2.34</v>
       </c>
       <c r="G82" s="19">
-        <f>$D82*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D82*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H82" s="20">
-        <f>$E82*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E82*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.90999999999999992</v>
       </c>
       <c r="I82" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>1.568312328767123</v>
       </c>
       <c r="J82" s="17">
-        <f>$D82*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D82*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K82" s="18">
-        <f>$E82*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E82*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.90999999999999992</v>
       </c>
       <c r="L82" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>1.2388849315068491</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="14">
-        <v>0.41666666666666702</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="B83" s="13">
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="C83" s="15">
         <f t="shared" si="5"/>
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="D83" s="15">
         <f t="shared" si="6"/>
@@ -5881,40 +5985,40 @@
       </c>
       <c r="E83" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="F83" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C83</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C83</f>
+        <v>1.95</v>
       </c>
       <c r="G83" s="19">
-        <f>$D83*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D83*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H83" s="20">
-        <f>$E83*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E83*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.52</v>
       </c>
       <c r="I83" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>1.1783123287671233</v>
       </c>
       <c r="J83" s="17">
-        <f>$D83*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D83*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K83" s="18">
-        <f>$E83*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E83*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.52</v>
       </c>
       <c r="L83" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.84888493150684929</v>
       </c>
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="14">
-        <v>0.45833333333333298</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="B84" s="13">
         <v>1100</v>
@@ -5932,37 +6036,37 @@
         <v>0</v>
       </c>
       <c r="F84" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C84</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C84</f>
+        <v>1.43</v>
       </c>
       <c r="G84" s="19">
-        <f>$D84*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D84*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H84" s="20">
-        <f>$E84*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E84*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I84" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J84" s="17">
-        <f>$D84*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D84*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K84" s="18">
-        <f>$E84*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E84*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L84" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="14">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="B85" s="13">
         <v>1100</v>
@@ -5980,37 +6084,37 @@
         <v>0</v>
       </c>
       <c r="F85" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C85</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C85</f>
+        <v>1.43</v>
       </c>
       <c r="G85" s="19">
-        <f>$D85*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D85*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H85" s="20">
-        <f>$E85*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E85*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I85" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J85" s="17">
-        <f>$D85*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D85*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K85" s="18">
-        <f>$E85*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E85*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L85" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="14">
-        <v>0.54166666666666696</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="B86" s="13">
         <v>1100</v>
@@ -6028,44 +6132,44 @@
         <v>0</v>
       </c>
       <c r="F86" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C86</f>
-        <v>0.28599999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C86</f>
+        <v>1.43</v>
       </c>
       <c r="G86" s="19">
-        <f>$D86*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D86*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H86" s="20">
-        <f>$E86*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E86*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I86" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J86" s="17">
-        <f>$D86*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D86*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K86" s="18">
-        <f>$E86*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E86*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L86" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="14">
-        <v>0.58333333333333304</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="B87" s="13">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="C87" s="15">
         <f t="shared" si="5"/>
-        <v>4000</v>
+        <v>2200</v>
       </c>
       <c r="D87" s="15">
         <f t="shared" si="6"/>
@@ -6073,47 +6177,47 @@
       </c>
       <c r="E87" s="15">
         <f t="shared" si="7"/>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="F87" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C87</f>
-        <v>0.51999999999999991</v>
+        <f>'Pricing (us-west-2)'!$B$5*C87</f>
+        <v>1.43</v>
       </c>
       <c r="G87" s="19">
-        <f>$D87*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D87*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H87" s="20">
-        <f>$E87*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.23399999999999999</v>
+        <f>$E87*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I87" s="19">
         <f t="shared" si="8"/>
-        <v>0.36434246575342466</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J87" s="17">
-        <f>$D87*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D87*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K87" s="18">
-        <f>$E87*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.23399999999999999</v>
+        <f>$E87*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L87" s="17">
         <f t="shared" si="9"/>
-        <v>0.29933698630136985</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="14">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="B88" s="13">
-        <v>2200</v>
+        <v>1100</v>
       </c>
       <c r="C88" s="15">
         <f t="shared" si="5"/>
-        <v>4400</v>
+        <v>2200</v>
       </c>
       <c r="D88" s="15">
         <f t="shared" si="6"/>
@@ -6121,47 +6225,47 @@
       </c>
       <c r="E88" s="15">
         <f t="shared" si="7"/>
-        <v>2200</v>
+        <v>0</v>
       </c>
       <c r="F88" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C88</f>
-        <v>0.57199999999999995</v>
+        <f>'Pricing (us-west-2)'!$B$5*C88</f>
+        <v>1.43</v>
       </c>
       <c r="G88" s="19">
-        <f>$D88*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D88*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H88" s="20">
-        <f>$E88*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.28599999999999998</v>
+        <f>$E88*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I88" s="19">
         <f t="shared" si="8"/>
-        <v>0.41634246575342465</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J88" s="17">
-        <f>$D88*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D88*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K88" s="18">
-        <f>$E88*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.28599999999999998</v>
+        <f>$E88*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L88" s="17">
         <f t="shared" si="9"/>
-        <v>0.35133698630136984</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="14">
-        <v>0.66666666666666696</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="B89" s="13">
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="C89" s="15">
         <f t="shared" si="5"/>
-        <v>5000</v>
+        <v>2200</v>
       </c>
       <c r="D89" s="15">
         <f t="shared" si="6"/>
@@ -6169,40 +6273,40 @@
       </c>
       <c r="E89" s="15">
         <f t="shared" si="7"/>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="F89" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C89</f>
-        <v>0.64999999999999991</v>
+        <f>'Pricing (us-west-2)'!$B$5*C89</f>
+        <v>1.43</v>
       </c>
       <c r="G89" s="19">
-        <f>$D89*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D89*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H89" s="20">
-        <f>$E89*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.36399999999999999</v>
+        <f>$E89*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="I89" s="19">
         <f t="shared" si="8"/>
-        <v>0.49434246575342466</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J89" s="17">
-        <f>$D89*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D89*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K89" s="18">
-        <f>$E89*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.36399999999999999</v>
+        <f>$E89*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
       </c>
       <c r="L89" s="17">
         <f t="shared" si="9"/>
-        <v>0.42933698630136985</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="14">
-        <v>0.70833333333333304</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="B90" s="13">
         <v>2000</v>
@@ -6220,44 +6324,44 @@
         <v>1800</v>
       </c>
       <c r="F90" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C90</f>
-        <v>0.51999999999999991</v>
+        <f>'Pricing (us-west-2)'!$B$5*C90</f>
+        <v>2.6</v>
       </c>
       <c r="G90" s="19">
-        <f>$D90*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D90*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H90" s="20">
-        <f>$E90*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.23399999999999999</v>
+        <f>$E90*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.17</v>
       </c>
       <c r="I90" s="19">
         <f t="shared" si="8"/>
-        <v>0.36434246575342466</v>
+        <v>1.8283123287671232</v>
       </c>
       <c r="J90" s="17">
-        <f>$D90*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D90*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K90" s="18">
-        <f>$E90*'Pricing (us-west-2)'!$C$5</f>
-        <v>0.23399999999999999</v>
+        <f>$E90*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.17</v>
       </c>
       <c r="L90" s="17">
         <f t="shared" si="9"/>
-        <v>0.29933698630136985</v>
+        <v>1.4988849315068493</v>
       </c>
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="14">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="B91" s="13">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C91" s="15">
         <f t="shared" si="5"/>
-        <v>2400</v>
+        <v>4400</v>
       </c>
       <c r="D91" s="15">
         <f t="shared" si="6"/>
@@ -6265,47 +6369,47 @@
       </c>
       <c r="E91" s="15">
         <f t="shared" si="7"/>
-        <v>200</v>
+        <v>2200</v>
       </c>
       <c r="F91" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C91</f>
-        <v>0.312</v>
+        <f>'Pricing (us-west-2)'!$B$5*C91</f>
+        <v>2.86</v>
       </c>
       <c r="G91" s="19">
-        <f>$D91*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D91*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H91" s="20">
-        <f>$E91*'Pricing (us-west-2)'!$C$5</f>
-        <v>2.5999999999999999E-2</v>
+        <f>$E91*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.43</v>
       </c>
       <c r="I91" s="19">
         <f t="shared" si="8"/>
-        <v>0.15634246575342467</v>
+        <v>2.088312328767123</v>
       </c>
       <c r="J91" s="17">
-        <f>$D91*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D91*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K91" s="18">
-        <f>$E91*'Pricing (us-west-2)'!$C$5</f>
-        <v>2.5999999999999999E-2</v>
+        <f>$E91*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.43</v>
       </c>
       <c r="L91" s="17">
         <f t="shared" si="9"/>
-        <v>9.1336986301369869E-2</v>
+        <v>1.7588849315068491</v>
       </c>
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="14">
-        <v>0.79166666666666696</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="B92" s="13">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C92" s="15">
         <f t="shared" si="5"/>
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="D92" s="15">
         <f t="shared" si="6"/>
@@ -6313,47 +6417,47 @@
       </c>
       <c r="E92" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2800</v>
       </c>
       <c r="F92" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C92</f>
-        <v>0.25999999999999995</v>
+        <f>'Pricing (us-west-2)'!$B$5*C92</f>
+        <v>3.25</v>
       </c>
       <c r="G92" s="19">
-        <f>$D92*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D92*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H92" s="20">
-        <f>$E92*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E92*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.8199999999999998</v>
       </c>
       <c r="I92" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>2.4783123287671232</v>
       </c>
       <c r="J92" s="17">
-        <f>$D92*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D92*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K92" s="18">
-        <f>$E92*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E92*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.8199999999999998</v>
       </c>
       <c r="L92" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>2.1488849315068492</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="14">
-        <v>0.83333333333333304</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="B93" s="13">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="C93" s="15">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="D93" s="15">
         <f t="shared" si="6"/>
@@ -6361,47 +6465,47 @@
       </c>
       <c r="E93" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="F93" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C93</f>
-        <v>0.12999999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C93</f>
+        <v>2.6</v>
       </c>
       <c r="G93" s="19">
-        <f>$D93*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D93*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H93" s="20">
-        <f>$E93*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E93*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.17</v>
       </c>
       <c r="I93" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>1.8283123287671232</v>
       </c>
       <c r="J93" s="17">
-        <f>$D93*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D93*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K93" s="18">
-        <f>$E93*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E93*'Pricing (us-west-2)'!$B$5</f>
+        <v>1.17</v>
       </c>
       <c r="L93" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>1.4988849315068493</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="14">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="B94" s="13">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="C94" s="15">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>2400</v>
       </c>
       <c r="D94" s="15">
         <f t="shared" si="6"/>
@@ -6409,47 +6513,47 @@
       </c>
       <c r="E94" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F94" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C94</f>
-        <v>0.12999999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C94</f>
+        <v>1.5599999999999998</v>
       </c>
       <c r="G94" s="19">
-        <f>$D94*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D94*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H94" s="20">
-        <f>$E94*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E94*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.13</v>
       </c>
       <c r="I94" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.7883123287671232</v>
       </c>
       <c r="J94" s="17">
-        <f>$D94*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D94*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K94" s="18">
-        <f>$E94*'Pricing (us-west-2)'!$C$5</f>
-        <v>0</v>
+        <f>$E94*'Pricing (us-west-2)'!$B$5</f>
+        <v>0.13</v>
       </c>
       <c r="L94" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.45888493150684928</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="14">
-        <v>0.91666666666666596</v>
+        <v>0.79166666666666696</v>
       </c>
       <c r="B95" s="13">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C95" s="15">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D95" s="15">
         <f t="shared" si="6"/>
@@ -6460,37 +6564,37 @@
         <v>0</v>
       </c>
       <c r="F95" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C95</f>
-        <v>0.12999999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C95</f>
+        <v>1.3</v>
       </c>
       <c r="G95" s="19">
-        <f>$D95*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D95*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H95" s="20">
-        <f>$E95*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E95*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I95" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J95" s="17">
-        <f>$D95*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D95*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K95" s="18">
-        <f>$E95*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E95*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L95" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="14">
-        <v>0.95833333333333304</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="B96" s="13">
         <v>500</v>
@@ -6508,44 +6612,44 @@
         <v>0</v>
       </c>
       <c r="F96" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C96</f>
-        <v>0.12999999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C96</f>
+        <v>0.65</v>
       </c>
       <c r="G96" s="19">
-        <f>$D96*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D96*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H96" s="20">
-        <f>$E96*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E96*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I96" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J96" s="17">
-        <f>$D96*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D96*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K96" s="18">
-        <f>$E96*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E96*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L96" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="14">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="B97" s="13">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="C97" s="15">
         <f t="shared" si="5"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="D97" s="15">
         <f t="shared" si="6"/>
@@ -6556,128 +6660,336 @@
         <v>0</v>
       </c>
       <c r="F97" s="21">
-        <f>'Pricing (us-west-2)'!$C$5*C97</f>
-        <v>0.19499999999999998</v>
+        <f>'Pricing (us-west-2)'!$B$5*C97</f>
+        <v>0.65</v>
       </c>
       <c r="G97" s="19">
-        <f>$D97*'Pricing (us-west-2)'!$C$6</f>
-        <v>0.13034246575342467</v>
+        <f>$D97*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
       </c>
       <c r="H97" s="20">
-        <f>$E97*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E97*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="I97" s="19">
         <f t="shared" si="8"/>
-        <v>0.13034246575342467</v>
+        <v>0.6583123287671232</v>
       </c>
       <c r="J97" s="17">
-        <f>$D97*'Pricing (us-west-2)'!$C$7</f>
-        <v>6.5336986301369873E-2</v>
+        <f>$D97*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
       </c>
       <c r="K97" s="18">
-        <f>$E97*'Pricing (us-west-2)'!$C$5</f>
+        <f>$E97*'Pricing (us-west-2)'!$B$5</f>
         <v>0</v>
       </c>
       <c r="L97" s="17">
         <f t="shared" si="9"/>
-        <v>6.5336986301369873E-2</v>
+        <v>0.32888493150684928</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="14">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="B98" s="13">
+        <v>500</v>
+      </c>
+      <c r="C98" s="15">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="D98" s="15">
+        <f t="shared" si="6"/>
+        <v>2200</v>
+      </c>
+      <c r="E98" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="21">
+        <f>'Pricing (us-west-2)'!$B$5*C98</f>
+        <v>0.65</v>
+      </c>
+      <c r="G98" s="19">
+        <f>$D98*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="H98" s="20">
+        <f>$E98*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="I98" s="19">
+        <f t="shared" si="8"/>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="J98" s="17">
+        <f>$D98*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
+      </c>
+      <c r="K98" s="18">
+        <f>$E98*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="L98" s="17">
+        <f t="shared" si="9"/>
+        <v>0.32888493150684928</v>
       </c>
     </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="14">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B99" s="13">
+        <v>500</v>
+      </c>
+      <c r="C99" s="15">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="D99" s="15">
+        <f t="shared" si="6"/>
+        <v>2200</v>
+      </c>
+      <c r="E99" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="21">
+        <f>'Pricing (us-west-2)'!$B$5*C99</f>
+        <v>0.65</v>
+      </c>
+      <c r="G99" s="19">
+        <f>$D99*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="H99" s="20">
+        <f>$E99*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="I99" s="19">
+        <f t="shared" si="8"/>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="J99" s="17">
+        <f>$D99*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
+      </c>
+      <c r="K99" s="18">
+        <f>$E99*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="L99" s="17">
+        <f t="shared" si="9"/>
+        <v>0.32888493150684928</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="14">
+        <v>1</v>
+      </c>
+      <c r="B100" s="13">
+        <v>750</v>
+      </c>
+      <c r="C100" s="15">
+        <f t="shared" si="5"/>
+        <v>1500</v>
+      </c>
+      <c r="D100" s="15">
+        <f t="shared" si="6"/>
+        <v>2200</v>
+      </c>
+      <c r="E100" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F100" s="21">
+        <f>'Pricing (us-west-2)'!$B$5*C100</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G100" s="19">
+        <f>$D100*'Pricing (us-west-2)'!$B$6</f>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="H100" s="20">
+        <f>$E100*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="I100" s="19">
+        <f t="shared" si="8"/>
+        <v>0.6583123287671232</v>
+      </c>
+      <c r="J100" s="17">
+        <f>$D100*'Pricing (us-west-2)'!$B$7</f>
+        <v>0.32888493150684928</v>
+      </c>
+      <c r="K100" s="18">
+        <f>$E100*'Pricing (us-west-2)'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="L100" s="17">
+        <f t="shared" si="9"/>
+        <v>0.32888493150684928</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B99" s="76">
-        <f>AVERAGE(B74:B97)</f>
+      <c r="B102" s="68">
+        <f>AVERAGE(B77:B100)</f>
         <v>1227.0833333333333</v>
       </c>
-      <c r="C99" s="76">
-        <f>AVERAGE(C74:C97)</f>
+      <c r="C102" s="68">
+        <f>AVERAGE(C77:C100)</f>
         <v>2454.1666666666665</v>
       </c>
-      <c r="D99" s="76">
-        <f>AVERAGE(D74:D97)</f>
+      <c r="D102" s="68">
+        <f>AVERAGE(D77:D100)</f>
         <v>2200</v>
       </c>
-      <c r="E99" s="76">
-        <f>AVERAGE(E74:E97)</f>
+      <c r="E102" s="68">
+        <f>AVERAGE(E77:E100)</f>
         <v>491.66666666666669</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
-      <c r="A101" s="22" t="s">
+    <row r="104" spans="1:12">
+      <c r="A104" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B101" s="22"/>
-      <c r="C101" s="22"/>
-      <c r="D101" s="22"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="22">
-        <f>SUM(F74:F97)</f>
-        <v>7.6569999999999991</v>
-      </c>
-      <c r="G101" s="22"/>
-      <c r="H101" s="22" t="s">
+      <c r="B104" s="22"/>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22">
+        <f>SUM(F77:F100)</f>
+        <v>38.284999999999997</v>
+      </c>
+      <c r="G104" s="22"/>
+      <c r="H104" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I101" s="22">
-        <f>SUM(I74:I97)</f>
-        <v>4.6622191780821938</v>
-      </c>
-      <c r="J101" s="22"/>
-      <c r="K101" s="22" t="s">
+      <c r="I104" s="22">
+        <f>SUM(I77:I100)</f>
+        <v>23.469495890410961</v>
+      </c>
+      <c r="J104" s="22"/>
+      <c r="K104" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="L101" s="22">
-        <f>SUM(L74:L97)</f>
-        <v>3.102087671232876</v>
+      <c r="L104" s="22">
+        <f>SUM(L77:L100)</f>
+        <v>15.563238356164378</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="J72:L72"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:E42"/>
   </mergeCells>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="35" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -6685,7 +6997,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="E39">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -6693,7 +7005,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
+  <conditionalFormatting sqref="G38">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -6701,7 +7013,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
+  <conditionalFormatting sqref="G39">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -6718,8 +7030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DC622B-C311-0242-AF66-B192A16E8A25}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>